<commit_message>
Add appnotes and fix power budget
New application notes related to uC quiescent current and PCB antennas
added. Power budget now includes current and power draw for two new
uC-radio configurations.
</commit_message>
<xml_diff>
--- a/specs/base-power_budget.xlsx
+++ b/specs/base-power_budget.xlsx
@@ -5,14 +5,16 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jzheng13\Documents\HA-HA\specs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jzheng13\Documents\hardware\specs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8085"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Kinetis-Atmel" sheetId="1" r:id="rId1"/>
+    <sheet name="Kinetis-XBee" sheetId="2" r:id="rId2"/>
+    <sheet name="Atmel-Atmel" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="38">
   <si>
     <t>V_CC (V)</t>
   </si>
@@ -108,6 +110,36 @@
   </si>
   <si>
     <t>Max Power (Typical Voltage)</t>
+  </si>
+  <si>
+    <t>XBee-Pro 900HP 900MHz Antenna RX</t>
+  </si>
+  <si>
+    <t>XBee-Pro 900HP 900MHz Antenna Standby</t>
+  </si>
+  <si>
+    <t>XBee-Pro 900HP 900MHz Antenna TX</t>
+  </si>
+  <si>
+    <t>Atmel SAMB11 uC only</t>
+  </si>
+  <si>
+    <t>Atmel SAMB11 RX</t>
+  </si>
+  <si>
+    <t>Atmel SAMB11 TX</t>
+  </si>
+  <si>
+    <t>Atmel SAMB11 Standby</t>
+  </si>
+  <si>
+    <t>Send 2 second "keep-alive" signal every 10 seconds. Using +0dBm mode.</t>
+  </si>
+  <si>
+    <t>Using +3dBm mode.</t>
+  </si>
+  <si>
+    <t>Max</t>
   </si>
 </sst>
 </file>
@@ -451,9 +483,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -528,7 +558,7 @@
         <v>6.76</v>
       </c>
       <c r="E4" s="2">
-        <f>C4*D4</f>
+        <f t="shared" ref="E4:E12" si="0">C4*D4</f>
         <v>22.308</v>
       </c>
       <c r="F4" s="4">
@@ -536,7 +566,7 @@
         <v>0.2</v>
       </c>
       <c r="G4" s="2">
-        <f t="shared" ref="G4:G14" si="0">E4*F4</f>
+        <f t="shared" ref="G4:G14" si="1">E4*F4</f>
         <v>4.4615999999999998</v>
       </c>
       <c r="I4" s="2" t="s">
@@ -554,7 +584,7 @@
         <v>6.08</v>
       </c>
       <c r="E5" s="2">
-        <f t="shared" ref="E5:E10" si="1">C5*D5</f>
+        <f t="shared" si="0"/>
         <v>20.064</v>
       </c>
       <c r="F5" s="4">
@@ -562,7 +592,7 @@
         <v>0.2</v>
       </c>
       <c r="G5" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.0128000000000004</v>
       </c>
       <c r="I5" s="2" t="s">
@@ -580,7 +610,7 @@
         <v>0.2</v>
       </c>
       <c r="E6" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.66</v>
       </c>
       <c r="F6" s="4">
@@ -588,7 +618,7 @@
         <v>0.60000000000000009</v>
       </c>
       <c r="G6" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.39600000000000007</v>
       </c>
     </row>
@@ -603,7 +633,7 @@
         <v>9.1999999999999993</v>
       </c>
       <c r="E7" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>27.599999999999998</v>
       </c>
       <c r="F7" s="4">
@@ -611,7 +641,7 @@
         <v>0.99444444444444446</v>
       </c>
       <c r="G7" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>27.446666666666665</v>
       </c>
       <c r="I7" s="2" t="s">
@@ -629,6 +659,7 @@
         <v>23</v>
       </c>
       <c r="E8" s="2">
+        <f t="shared" si="0"/>
         <v>69</v>
       </c>
       <c r="F8" s="4">
@@ -636,7 +667,7 @@
         <v>5.5555555555555558E-3</v>
       </c>
       <c r="G8" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.38333333333333336</v>
       </c>
       <c r="I8" s="2" t="s">
@@ -654,7 +685,7 @@
         <v>0.45</v>
       </c>
       <c r="E9" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.35</v>
       </c>
       <c r="F9" s="4">
@@ -662,7 +693,7 @@
         <v>0</v>
       </c>
       <c r="G9" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -677,14 +708,14 @@
         <v>0.03</v>
       </c>
       <c r="E10" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>5.3999999999999999E-2</v>
       </c>
       <c r="F10" s="4">
         <v>0.05</v>
       </c>
       <c r="G10" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.7000000000000001E-3</v>
       </c>
     </row>
@@ -699,14 +730,14 @@
         <v>1.2</v>
       </c>
       <c r="E11" s="2">
-        <f>C11*D11</f>
+        <f t="shared" si="0"/>
         <v>3.9599999999999995</v>
       </c>
       <c r="F11" s="4">
         <v>0.05</v>
       </c>
       <c r="G11" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.19799999999999998</v>
       </c>
     </row>
@@ -721,14 +752,14 @@
         <v>220</v>
       </c>
       <c r="E12" s="2">
-        <f>C12*D12</f>
+        <f t="shared" si="0"/>
         <v>924</v>
       </c>
       <c r="F12" s="4">
         <v>0.05</v>
       </c>
       <c r="G12" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>46.2</v>
       </c>
     </row>
@@ -749,7 +780,7 @@
         <v>0.01</v>
       </c>
       <c r="G13" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.4</v>
       </c>
       <c r="I13" s="2" t="s">
@@ -767,12 +798,21 @@
         <v>0.01</v>
       </c>
       <c r="G14" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
     </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="2">
+        <f>SUM(D3:D14)</f>
+        <v>292.52</v>
+      </c>
+    </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D16" s="1" t="s">
+      <c r="B16" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E16" s="2">
@@ -784,6 +824,9 @@
         <v>112.9811</v>
       </c>
     </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D17" s="1"/>
+    </row>
     <row r="18" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>27</v>
@@ -843,7 +886,7 @@
         <v>6.76</v>
       </c>
       <c r="E21" s="2">
-        <f>C21*D21</f>
+        <f t="shared" ref="E21:E29" si="2">C21*D21</f>
         <v>22.308</v>
       </c>
       <c r="F21" s="4">
@@ -851,7 +894,7 @@
         <v>0.5</v>
       </c>
       <c r="G21" s="2">
-        <f t="shared" ref="G21:G31" si="2">E21*F21</f>
+        <f t="shared" ref="G21:G31" si="3">E21*F21</f>
         <v>11.154</v>
       </c>
     </row>
@@ -866,14 +909,14 @@
         <v>6.08</v>
       </c>
       <c r="E22" s="2">
-        <f t="shared" ref="E22:E24" si="3">C22*D22</f>
+        <f t="shared" si="2"/>
         <v>20.064</v>
       </c>
       <c r="F22" s="4">
         <v>0.5</v>
       </c>
       <c r="G22" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>10.032</v>
       </c>
     </row>
@@ -888,7 +931,7 @@
         <v>0.2</v>
       </c>
       <c r="E23" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.66</v>
       </c>
       <c r="F23" s="4">
@@ -896,7 +939,7 @@
         <v>0</v>
       </c>
       <c r="G23" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -911,7 +954,7 @@
         <v>9.1999999999999993</v>
       </c>
       <c r="E24" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>27.599999999999998</v>
       </c>
       <c r="F24" s="4">
@@ -919,7 +962,7 @@
         <v>0.5</v>
       </c>
       <c r="G24" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>13.799999999999999</v>
       </c>
     </row>
@@ -934,14 +977,15 @@
         <v>31.5</v>
       </c>
       <c r="E25" s="2">
-        <v>69</v>
+        <f t="shared" si="2"/>
+        <v>94.5</v>
       </c>
       <c r="F25" s="4">
         <v>0.5</v>
       </c>
       <c r="G25" s="2">
-        <f t="shared" si="2"/>
-        <v>34.5</v>
+        <f t="shared" si="3"/>
+        <v>47.25</v>
       </c>
       <c r="I25" s="2" t="s">
         <v>20</v>
@@ -958,7 +1002,7 @@
         <v>0.45</v>
       </c>
       <c r="E26" s="2">
-        <f t="shared" ref="E26:E27" si="4">C26*D26</f>
+        <f t="shared" si="2"/>
         <v>1.35</v>
       </c>
       <c r="F26" s="4">
@@ -966,7 +1010,7 @@
         <v>0</v>
       </c>
       <c r="G26" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -981,14 +1025,14 @@
         <v>0.03</v>
       </c>
       <c r="E27" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>5.3999999999999999E-2</v>
       </c>
       <c r="F27" s="4">
         <v>1</v>
       </c>
       <c r="G27" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.3999999999999999E-2</v>
       </c>
     </row>
@@ -1003,14 +1047,14 @@
         <v>1.2</v>
       </c>
       <c r="E28" s="2">
-        <f>C28*D28</f>
+        <f t="shared" si="2"/>
         <v>3.9599999999999995</v>
       </c>
       <c r="F28" s="4">
         <v>1</v>
       </c>
       <c r="G28" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.9599999999999995</v>
       </c>
     </row>
@@ -1025,14 +1069,14 @@
         <v>220</v>
       </c>
       <c r="E29" s="2">
-        <f>C29*D29</f>
+        <f t="shared" si="2"/>
         <v>924</v>
       </c>
       <c r="F29" s="4">
         <v>1</v>
       </c>
       <c r="G29" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>924</v>
       </c>
     </row>
@@ -1053,7 +1097,7 @@
         <v>1</v>
       </c>
       <c r="G30" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>640</v>
       </c>
       <c r="I30" s="2" t="s">
@@ -1071,21 +1115,30 @@
         <v>1</v>
       </c>
       <c r="G31" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>500</v>
       </c>
     </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B32" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D32" s="2">
+        <f>SUM(D20:D31)</f>
+        <v>304.06</v>
+      </c>
+    </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D33" s="1" t="s">
+      <c r="B33" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E33" s="2">
         <f>SUM(E20:E31)</f>
-        <v>2237.5079999999998</v>
+        <v>2263.0079999999998</v>
       </c>
       <c r="G33" s="2">
         <f>SUM(G20:G31)</f>
-        <v>2166.0119999999997</v>
+        <v>2178.7619999999997</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -1156,7 +1209,7 @@
         <v>6.76</v>
       </c>
       <c r="E38" s="2">
-        <f>C38*D38</f>
+        <f t="shared" ref="E38:E46" si="4">C38*D38</f>
         <v>28.391999999999999</v>
       </c>
       <c r="F38" s="4">
@@ -1179,7 +1232,7 @@
         <v>6.08</v>
       </c>
       <c r="E39" s="2">
-        <f t="shared" ref="E39:E41" si="6">C39*D39</f>
+        <f t="shared" si="4"/>
         <v>25.536000000000001</v>
       </c>
       <c r="F39" s="4">
@@ -1201,7 +1254,7 @@
         <v>0.2</v>
       </c>
       <c r="E40" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.84000000000000008</v>
       </c>
       <c r="F40" s="4">
@@ -1224,7 +1277,7 @@
         <v>9.1999999999999993</v>
       </c>
       <c r="E41" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>33.119999999999997</v>
       </c>
       <c r="F41" s="4">
@@ -1247,14 +1300,15 @@
         <v>31.5</v>
       </c>
       <c r="E42" s="2">
-        <v>69</v>
+        <f t="shared" si="4"/>
+        <v>113.4</v>
       </c>
       <c r="F42" s="4">
         <v>0.5</v>
       </c>
       <c r="G42" s="2">
         <f t="shared" si="5"/>
-        <v>34.5</v>
+        <v>56.7</v>
       </c>
       <c r="I42" s="2" t="s">
         <v>20</v>
@@ -1271,7 +1325,7 @@
         <v>0.45</v>
       </c>
       <c r="E43" s="2">
-        <f t="shared" ref="E43:E44" si="7">C43*D43</f>
+        <f t="shared" si="4"/>
         <v>1.62</v>
       </c>
       <c r="F43" s="4">
@@ -1294,7 +1348,7 @@
         <v>0.03</v>
       </c>
       <c r="E44" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>5.9399999999999994E-2</v>
       </c>
       <c r="F44" s="4">
@@ -1316,7 +1370,7 @@
         <v>1.2</v>
       </c>
       <c r="E45" s="2">
-        <f>C45*D45</f>
+        <f t="shared" si="4"/>
         <v>5.3999999999999995</v>
       </c>
       <c r="F45" s="4">
@@ -1338,7 +1392,7 @@
         <v>220</v>
       </c>
       <c r="E46" s="2">
-        <f>C46*D46</f>
+        <f t="shared" si="4"/>
         <v>990</v>
       </c>
       <c r="F46" s="4">
@@ -1388,21 +1442,1709 @@
         <v>500</v>
       </c>
     </row>
-    <row r="50" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D50" s="1" t="s">
+    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B49" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D49" s="2">
+        <f>SUM(D37:D48)</f>
+        <v>304.06</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B50" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E50" s="2">
         <f>SUM(E37:E48)</f>
-        <v>2330.2554</v>
+        <v>2374.6554000000001</v>
       </c>
       <c r="G50" s="2">
         <f>SUM(G37:G48)</f>
-        <v>2249.7714000000001</v>
+        <v>2271.9713999999999</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I50"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="43" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="2"/>
+    <col min="3" max="3" width="8.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="2"/>
+    <col min="9" max="9" width="66.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="3"/>
+    </row>
+    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="2">
+        <v>3.3</v>
+      </c>
+      <c r="D3" s="2">
+        <v>5.6</v>
+      </c>
+      <c r="E3" s="2">
+        <f>C3*D3</f>
+        <v>18.479999999999997</v>
+      </c>
+      <c r="F3" s="4">
+        <v>1</v>
+      </c>
+      <c r="G3" s="2">
+        <f>E3*F3</f>
+        <v>18.479999999999997</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="2">
+        <v>3.3</v>
+      </c>
+      <c r="D4" s="2">
+        <v>6.76</v>
+      </c>
+      <c r="E4" s="2">
+        <f t="shared" ref="E4:E12" si="0">C4*D4</f>
+        <v>22.308</v>
+      </c>
+      <c r="F4" s="4">
+        <f>F5</f>
+        <v>0.2</v>
+      </c>
+      <c r="G4" s="2">
+        <f t="shared" ref="G4:G14" si="1">E4*F4</f>
+        <v>4.4615999999999998</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="2">
+        <v>3.3</v>
+      </c>
+      <c r="D5" s="2">
+        <v>6.08</v>
+      </c>
+      <c r="E5" s="2">
+        <f t="shared" si="0"/>
+        <v>20.064</v>
+      </c>
+      <c r="F5" s="4">
+        <f>2/10</f>
+        <v>0.2</v>
+      </c>
+      <c r="G5" s="2">
+        <f t="shared" si="1"/>
+        <v>4.0128000000000004</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="2">
+        <v>3.3</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="E6" s="2">
+        <f t="shared" si="0"/>
+        <v>0.66</v>
+      </c>
+      <c r="F6" s="4">
+        <f>1-F4-F5</f>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="G6" s="2">
+        <f t="shared" si="1"/>
+        <v>0.39600000000000007</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="2">
+        <v>3.3</v>
+      </c>
+      <c r="D7" s="2">
+        <v>44</v>
+      </c>
+      <c r="E7" s="2">
+        <f t="shared" si="0"/>
+        <v>145.19999999999999</v>
+      </c>
+      <c r="F7" s="4">
+        <f>1-F8</f>
+        <v>0.99444444444444446</v>
+      </c>
+      <c r="G7" s="2">
+        <f t="shared" si="1"/>
+        <v>144.39333333333332</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="2">
+        <v>3.3</v>
+      </c>
+      <c r="D8" s="2">
+        <v>229</v>
+      </c>
+      <c r="E8" s="2">
+        <f t="shared" si="0"/>
+        <v>755.69999999999993</v>
+      </c>
+      <c r="F8" s="4">
+        <f>5/900</f>
+        <v>5.5555555555555558E-3</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" si="1"/>
+        <v>4.1983333333333333</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="2">
+        <v>3.3</v>
+      </c>
+      <c r="D9" s="2">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="E9" s="2">
+        <f t="shared" si="0"/>
+        <v>9.8999999999999991E-3</v>
+      </c>
+      <c r="F9" s="4">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="G9" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1.8</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="E10" s="2">
+        <f t="shared" si="0"/>
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="F10" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="G10" s="2">
+        <f t="shared" si="1"/>
+        <v>2.7000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="2">
+        <v>3.3</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="E11" s="2">
+        <f t="shared" si="0"/>
+        <v>3.9599999999999995</v>
+      </c>
+      <c r="F11" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="G11" s="2">
+        <f t="shared" si="1"/>
+        <v>0.19799999999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="2">
+        <v>4.2</v>
+      </c>
+      <c r="D12" s="2">
+        <v>220</v>
+      </c>
+      <c r="E12" s="2">
+        <f t="shared" si="0"/>
+        <v>924</v>
+      </c>
+      <c r="F12" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="G12" s="2">
+        <f t="shared" si="1"/>
+        <v>46.2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="2">
+        <v>2</v>
+      </c>
+      <c r="D13" s="2">
+        <v>20</v>
+      </c>
+      <c r="E13" s="2">
+        <v>640</v>
+      </c>
+      <c r="F13" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="G13" s="2">
+        <f t="shared" si="1"/>
+        <v>6.4</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="2">
+        <v>500</v>
+      </c>
+      <c r="F14" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="G14" s="2">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="2">
+        <f>SUM(D3:D14)</f>
+        <v>532.87299999999993</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" s="2">
+        <f>SUM(E3:E14)</f>
+        <v>3030.4358999999999</v>
+      </c>
+      <c r="G16" s="2">
+        <f>SUM(G3:G14)</f>
+        <v>233.74276666666665</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F18" s="3"/>
+    </row>
+    <row r="19" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="2">
+        <v>3.3</v>
+      </c>
+      <c r="D20" s="2">
+        <v>8.64</v>
+      </c>
+      <c r="E20" s="2">
+        <f>C20*D20</f>
+        <v>28.512</v>
+      </c>
+      <c r="F20" s="4">
+        <v>1</v>
+      </c>
+      <c r="G20" s="2">
+        <f>E20*F20</f>
+        <v>28.512</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="2">
+        <v>3.3</v>
+      </c>
+      <c r="D21" s="2">
+        <v>6.76</v>
+      </c>
+      <c r="E21" s="2">
+        <f t="shared" ref="E21:E29" si="2">C21*D21</f>
+        <v>22.308</v>
+      </c>
+      <c r="F21" s="4">
+        <f>F22</f>
+        <v>0.5</v>
+      </c>
+      <c r="G21" s="2">
+        <f t="shared" ref="G21:G31" si="3">E21*F21</f>
+        <v>11.154</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="2">
+        <v>3.3</v>
+      </c>
+      <c r="D22" s="2">
+        <v>6.08</v>
+      </c>
+      <c r="E22" s="2">
+        <f t="shared" si="2"/>
+        <v>20.064</v>
+      </c>
+      <c r="F22" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="G22" s="2">
+        <f t="shared" si="3"/>
+        <v>10.032</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="2">
+        <v>3.3</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="E23" s="2">
+        <f t="shared" si="2"/>
+        <v>0.66</v>
+      </c>
+      <c r="F23" s="4">
+        <f>1-F21-F22</f>
+        <v>0</v>
+      </c>
+      <c r="G23" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" s="2">
+        <v>3.6</v>
+      </c>
+      <c r="D24" s="2">
+        <v>44</v>
+      </c>
+      <c r="E24" s="2">
+        <f t="shared" si="2"/>
+        <v>158.4</v>
+      </c>
+      <c r="F24" s="4">
+        <f>1-F25</f>
+        <v>0.5</v>
+      </c>
+      <c r="G24" s="2">
+        <f t="shared" si="3"/>
+        <v>79.2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25" s="2">
+        <v>3.6</v>
+      </c>
+      <c r="D25" s="2">
+        <v>229</v>
+      </c>
+      <c r="E25" s="2">
+        <f t="shared" si="2"/>
+        <v>824.4</v>
+      </c>
+      <c r="F25" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="G25" s="2">
+        <f t="shared" si="3"/>
+        <v>412.2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" s="2">
+        <v>3.6</v>
+      </c>
+      <c r="D26" s="2">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="E26" s="2">
+        <f t="shared" si="2"/>
+        <v>1.0800000000000001E-2</v>
+      </c>
+      <c r="F26" s="4">
+        <f>1-F24-F25</f>
+        <v>0</v>
+      </c>
+      <c r="G26" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27" s="2">
+        <v>1.8</v>
+      </c>
+      <c r="D27" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="E27" s="2">
+        <f t="shared" si="2"/>
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="F27" s="4">
+        <v>1</v>
+      </c>
+      <c r="G27" s="2">
+        <f t="shared" si="3"/>
+        <v>5.3999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C28" s="2">
+        <v>3.3</v>
+      </c>
+      <c r="D28" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="E28" s="2">
+        <f t="shared" si="2"/>
+        <v>3.9599999999999995</v>
+      </c>
+      <c r="F28" s="4">
+        <v>1</v>
+      </c>
+      <c r="G28" s="2">
+        <f t="shared" si="3"/>
+        <v>3.9599999999999995</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C29" s="2">
+        <v>4.2</v>
+      </c>
+      <c r="D29" s="2">
+        <v>220</v>
+      </c>
+      <c r="E29" s="2">
+        <f t="shared" si="2"/>
+        <v>924</v>
+      </c>
+      <c r="F29" s="4">
+        <v>1</v>
+      </c>
+      <c r="G29" s="2">
+        <f t="shared" si="3"/>
+        <v>924</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C30" s="2">
+        <v>2</v>
+      </c>
+      <c r="D30" s="2">
+        <v>20</v>
+      </c>
+      <c r="E30" s="2">
+        <v>640</v>
+      </c>
+      <c r="F30" s="4">
+        <v>1</v>
+      </c>
+      <c r="G30" s="2">
+        <f t="shared" si="3"/>
+        <v>640</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E31" s="2">
+        <v>500</v>
+      </c>
+      <c r="F31" s="4">
+        <v>1</v>
+      </c>
+      <c r="G31" s="2">
+        <f t="shared" si="3"/>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B32" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D32" s="2">
+        <f>SUM(D20:D31)</f>
+        <v>535.91300000000001</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B33" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E33" s="2">
+        <f>SUM(E20:E31)</f>
+        <v>3122.3688000000002</v>
+      </c>
+      <c r="G33" s="2">
+        <f>SUM(G20:G31)</f>
+        <v>2609.1120000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+    </row>
+    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D50" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I50"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="43" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="2"/>
+    <col min="3" max="3" width="8.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="2"/>
+    <col min="9" max="9" width="66.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="3"/>
+    </row>
+    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="2">
+        <v>3.3</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.85</v>
+      </c>
+      <c r="E3" s="2">
+        <f>C3*D3</f>
+        <v>2.8049999999999997</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="G3" s="2">
+        <f>E3*F3</f>
+        <v>1.6829999999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="2">
+        <v>3.3</v>
+      </c>
+      <c r="D4" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="E4" s="2">
+        <f t="shared" ref="E4:E12" si="0">C4*D4</f>
+        <v>14.85</v>
+      </c>
+      <c r="F4" s="4">
+        <f>F5</f>
+        <v>0.2</v>
+      </c>
+      <c r="G4" s="2">
+        <f t="shared" ref="G4:G14" si="1">E4*F4</f>
+        <v>2.97</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="2">
+        <v>3.3</v>
+      </c>
+      <c r="D5" s="2">
+        <v>3</v>
+      </c>
+      <c r="E5" s="2">
+        <f t="shared" si="0"/>
+        <v>9.8999999999999986</v>
+      </c>
+      <c r="F5" s="4">
+        <f>2/10</f>
+        <v>0.2</v>
+      </c>
+      <c r="G5" s="2">
+        <f t="shared" si="1"/>
+        <v>1.9799999999999998</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="2">
+        <v>3.3</v>
+      </c>
+      <c r="D6" s="2">
+        <v>1.1000000000000001E-3</v>
+      </c>
+      <c r="E6" s="2">
+        <f t="shared" si="0"/>
+        <v>3.63E-3</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="2">
+        <v>3</v>
+      </c>
+      <c r="D7" s="2">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="E7" s="2">
+        <f t="shared" si="0"/>
+        <v>27.599999999999998</v>
+      </c>
+      <c r="F7" s="4">
+        <f>1-F8</f>
+        <v>0.99444444444444446</v>
+      </c>
+      <c r="G7" s="2">
+        <f t="shared" si="1"/>
+        <v>27.446666666666665</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="2">
+        <v>3</v>
+      </c>
+      <c r="D8" s="2">
+        <v>23</v>
+      </c>
+      <c r="E8" s="2">
+        <f t="shared" si="0"/>
+        <v>69</v>
+      </c>
+      <c r="F8" s="4">
+        <f>5/900</f>
+        <v>5.5555555555555558E-3</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" si="1"/>
+        <v>0.38333333333333336</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="2">
+        <v>3</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="E9" s="2">
+        <f t="shared" si="0"/>
+        <v>1.35</v>
+      </c>
+      <c r="F9" s="4">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="G9" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1.8</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="E10" s="2">
+        <f t="shared" si="0"/>
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="F10" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="G10" s="2">
+        <f t="shared" si="1"/>
+        <v>2.7000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="2">
+        <v>3.3</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="E11" s="2">
+        <f t="shared" si="0"/>
+        <v>3.9599999999999995</v>
+      </c>
+      <c r="F11" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="G11" s="2">
+        <f t="shared" si="1"/>
+        <v>0.19799999999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="2">
+        <v>4.2</v>
+      </c>
+      <c r="D12" s="2">
+        <v>220</v>
+      </c>
+      <c r="E12" s="2">
+        <f t="shared" si="0"/>
+        <v>924</v>
+      </c>
+      <c r="F12" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="G12" s="2">
+        <f t="shared" si="1"/>
+        <v>46.2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="2">
+        <v>2</v>
+      </c>
+      <c r="D13" s="2">
+        <v>20</v>
+      </c>
+      <c r="E13" s="2">
+        <v>640</v>
+      </c>
+      <c r="F13" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="G13" s="2">
+        <f t="shared" si="1"/>
+        <v>6.4</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="2">
+        <v>500</v>
+      </c>
+      <c r="F14" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="G14" s="2">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="2">
+        <f>SUM(D3:D14)</f>
+        <v>282.23110000000003</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" s="2">
+        <f>SUM(E3:E14)</f>
+        <v>2193.5226299999999</v>
+      </c>
+      <c r="G16" s="2">
+        <f>SUM(G3:G14)</f>
+        <v>92.2637</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F18" s="3"/>
+    </row>
+    <row r="19" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="2">
+        <v>3.3</v>
+      </c>
+      <c r="D20" s="2">
+        <v>0.85</v>
+      </c>
+      <c r="E20" s="2">
+        <f>C20*D20</f>
+        <v>2.8049999999999997</v>
+      </c>
+      <c r="F20" s="4">
+        <v>0</v>
+      </c>
+      <c r="G20" s="2">
+        <f>E20*F20</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="2">
+        <v>3.3</v>
+      </c>
+      <c r="D21" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="E21" s="2">
+        <f t="shared" ref="E21:E29" si="2">C21*D21</f>
+        <v>14.85</v>
+      </c>
+      <c r="F21" s="4">
+        <f>F22</f>
+        <v>0.5</v>
+      </c>
+      <c r="G21" s="2">
+        <f t="shared" ref="G21:G31" si="3">E21*F21</f>
+        <v>7.4249999999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" s="2">
+        <v>3.3</v>
+      </c>
+      <c r="D22" s="2">
+        <v>4</v>
+      </c>
+      <c r="E22" s="2">
+        <f t="shared" si="2"/>
+        <v>13.2</v>
+      </c>
+      <c r="F22" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="G22" s="2">
+        <f t="shared" si="3"/>
+        <v>6.6</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23" s="2">
+        <v>3.3</v>
+      </c>
+      <c r="D23" s="2">
+        <v>1.25E-3</v>
+      </c>
+      <c r="E23" s="2">
+        <f t="shared" si="2"/>
+        <v>4.1250000000000002E-3</v>
+      </c>
+      <c r="F23" s="4">
+        <f>1-F21-F22</f>
+        <v>0</v>
+      </c>
+      <c r="G23" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="2">
+        <v>3</v>
+      </c>
+      <c r="D24" s="2">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="E24" s="2">
+        <f t="shared" si="2"/>
+        <v>27.599999999999998</v>
+      </c>
+      <c r="F24" s="4">
+        <f>1-F25</f>
+        <v>0.5</v>
+      </c>
+      <c r="G24" s="2">
+        <f t="shared" si="3"/>
+        <v>13.799999999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" s="2">
+        <v>3</v>
+      </c>
+      <c r="D25" s="2">
+        <v>31.5</v>
+      </c>
+      <c r="E25" s="2">
+        <f t="shared" si="2"/>
+        <v>94.5</v>
+      </c>
+      <c r="F25" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="G25" s="2">
+        <f t="shared" si="3"/>
+        <v>47.25</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" s="2">
+        <v>3</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="E26" s="2">
+        <f t="shared" si="2"/>
+        <v>1.35</v>
+      </c>
+      <c r="F26" s="4">
+        <f>1-F24-F25</f>
+        <v>0</v>
+      </c>
+      <c r="G26" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27" s="2">
+        <v>1.8</v>
+      </c>
+      <c r="D27" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="E27" s="2">
+        <f t="shared" si="2"/>
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="F27" s="4">
+        <v>1</v>
+      </c>
+      <c r="G27" s="2">
+        <f t="shared" si="3"/>
+        <v>5.3999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C28" s="2">
+        <v>3.3</v>
+      </c>
+      <c r="D28" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="E28" s="2">
+        <f t="shared" si="2"/>
+        <v>3.9599999999999995</v>
+      </c>
+      <c r="F28" s="4">
+        <v>1</v>
+      </c>
+      <c r="G28" s="2">
+        <f t="shared" si="3"/>
+        <v>3.9599999999999995</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C29" s="2">
+        <v>4.2</v>
+      </c>
+      <c r="D29" s="2">
+        <v>220</v>
+      </c>
+      <c r="E29" s="2">
+        <f t="shared" si="2"/>
+        <v>924</v>
+      </c>
+      <c r="F29" s="4">
+        <v>1</v>
+      </c>
+      <c r="G29" s="2">
+        <f t="shared" si="3"/>
+        <v>924</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C30" s="2">
+        <v>2</v>
+      </c>
+      <c r="D30" s="2">
+        <v>20</v>
+      </c>
+      <c r="E30" s="2">
+        <v>640</v>
+      </c>
+      <c r="F30" s="4">
+        <v>1</v>
+      </c>
+      <c r="G30" s="2">
+        <f t="shared" si="3"/>
+        <v>640</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E31" s="2">
+        <v>500</v>
+      </c>
+      <c r="F31" s="4">
+        <v>1</v>
+      </c>
+      <c r="G31" s="2">
+        <f t="shared" si="3"/>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B32" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D32" s="2">
+        <f>SUM(D20:D31)</f>
+        <v>291.73124999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B33" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E33" s="2">
+        <f>SUM(E20:E31)</f>
+        <v>2222.3231249999999</v>
+      </c>
+      <c r="G33" s="2">
+        <f>SUM(G20:G31)</f>
+        <v>2143.0889999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B36" s="1"/>
+      <c r="C36" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C37" s="2">
+        <v>4.3</v>
+      </c>
+      <c r="D37" s="2">
+        <v>0.85</v>
+      </c>
+      <c r="E37" s="2">
+        <f>C37*D37</f>
+        <v>3.6549999999999998</v>
+      </c>
+      <c r="F37" s="4">
+        <v>0</v>
+      </c>
+      <c r="G37" s="2">
+        <f>E37*F37</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C38" s="2">
+        <v>4.3</v>
+      </c>
+      <c r="D38" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="E38" s="2">
+        <f t="shared" ref="E38:E46" si="4">C38*D38</f>
+        <v>19.349999999999998</v>
+      </c>
+      <c r="F38" s="4">
+        <f>F39</f>
+        <v>0.5</v>
+      </c>
+      <c r="G38" s="2">
+        <f t="shared" ref="G38:G48" si="5">E38*F38</f>
+        <v>9.6749999999999989</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C39" s="2">
+        <v>4.3</v>
+      </c>
+      <c r="D39" s="2">
+        <v>4</v>
+      </c>
+      <c r="E39" s="2">
+        <f t="shared" si="4"/>
+        <v>17.2</v>
+      </c>
+      <c r="F39" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="G39" s="2">
+        <f t="shared" si="5"/>
+        <v>8.6</v>
+      </c>
+      <c r="I39" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C40" s="2">
+        <v>4.3</v>
+      </c>
+      <c r="D40" s="2">
+        <v>1.25E-3</v>
+      </c>
+      <c r="E40" s="2">
+        <f t="shared" si="4"/>
+        <v>5.3749999999999996E-3</v>
+      </c>
+      <c r="F40" s="4">
+        <f>1-F38-F39</f>
+        <v>0</v>
+      </c>
+      <c r="G40" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C41" s="2">
+        <v>3.6</v>
+      </c>
+      <c r="D41" s="2">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="E41" s="2">
+        <f t="shared" si="4"/>
+        <v>33.119999999999997</v>
+      </c>
+      <c r="F41" s="4">
+        <f>1-F42</f>
+        <v>0.5</v>
+      </c>
+      <c r="G41" s="2">
+        <f t="shared" si="5"/>
+        <v>16.559999999999999</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C42" s="2">
+        <v>3.6</v>
+      </c>
+      <c r="D42" s="2">
+        <v>31.5</v>
+      </c>
+      <c r="E42" s="2">
+        <f t="shared" si="4"/>
+        <v>113.4</v>
+      </c>
+      <c r="F42" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="G42" s="2">
+        <f t="shared" si="5"/>
+        <v>56.7</v>
+      </c>
+      <c r="I42" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C43" s="2">
+        <v>3.6</v>
+      </c>
+      <c r="D43" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="E43" s="2">
+        <f t="shared" si="4"/>
+        <v>1.62</v>
+      </c>
+      <c r="F43" s="4">
+        <f>1-F41-F42</f>
+        <v>0</v>
+      </c>
+      <c r="G43" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C44" s="2">
+        <v>1.98</v>
+      </c>
+      <c r="D44" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="E44" s="2">
+        <f t="shared" si="4"/>
+        <v>5.9399999999999994E-2</v>
+      </c>
+      <c r="F44" s="4">
+        <v>1</v>
+      </c>
+      <c r="G44" s="2">
+        <f t="shared" si="5"/>
+        <v>5.9399999999999994E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C45" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="D45" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="E45" s="2">
+        <f t="shared" si="4"/>
+        <v>5.3999999999999995</v>
+      </c>
+      <c r="F45" s="4">
+        <v>1</v>
+      </c>
+      <c r="G45" s="2">
+        <f t="shared" si="5"/>
+        <v>5.3999999999999995</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C46" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="D46" s="2">
+        <v>220</v>
+      </c>
+      <c r="E46" s="2">
+        <f t="shared" si="4"/>
+        <v>990</v>
+      </c>
+      <c r="F46" s="4">
+        <v>1</v>
+      </c>
+      <c r="G46" s="2">
+        <f t="shared" si="5"/>
+        <v>990</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C47" s="2">
+        <v>2</v>
+      </c>
+      <c r="D47" s="2">
+        <v>20</v>
+      </c>
+      <c r="E47" s="2">
+        <v>640</v>
+      </c>
+      <c r="F47" s="4">
+        <v>1</v>
+      </c>
+      <c r="G47" s="2">
+        <f t="shared" si="5"/>
+        <v>640</v>
+      </c>
+      <c r="I47" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E48" s="2">
+        <v>500</v>
+      </c>
+      <c r="F48" s="4">
+        <v>1</v>
+      </c>
+      <c r="G48" s="2">
+        <f t="shared" si="5"/>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B49" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D49" s="2">
+        <f>SUM(D37:D48)</f>
+        <v>291.73124999999999</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B50" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E50" s="2">
+        <f>SUM(E37:E48)</f>
+        <v>2323.8097749999997</v>
+      </c>
+      <c r="G50" s="2">
+        <f>SUM(G37:G48)</f>
+        <v>2226.9944</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>